<commit_message>
restart my dream project on 05/22/2019, after two months break from my Marathon
</commit_message>
<xml_diff>
--- a/lib/pkmeta.xlsx
+++ b/lib/pkmeta.xlsx
@@ -8,25 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\QP Portal\LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F65F3C52-D0B7-4451-BA3D-798EEA6E76B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{78E060E9-D85D-4BE6-AFFE-9B11F7A7A63B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="nmdat" sheetId="8" r:id="rId1"/>
-    <sheet name="adsl" sheetId="2" r:id="rId2"/>
-    <sheet name="adex" sheetId="3" r:id="rId3"/>
-    <sheet name="adpc" sheetId="4" r:id="rId4"/>
-    <sheet name="adpx" sheetId="9" r:id="rId5"/>
-    <sheet name="convention" sheetId="10" r:id="rId6"/>
-    <sheet name="cheatsheet" sheetId="7" r:id="rId7"/>
+    <sheet name="adsl" sheetId="2" r:id="rId1"/>
+    <sheet name="adex" sheetId="3" r:id="rId2"/>
+    <sheet name="adpc" sheetId="4" r:id="rId3"/>
+    <sheet name="nmdat" sheetId="8" r:id="rId4"/>
+    <sheet name="convention" sheetId="10" r:id="rId5"/>
+    <sheet name="cheatsheet" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="238">
   <si>
     <t>STUDYID</t>
   </si>
@@ -409,9 +408,6 @@
     <t>Unique subject identifier</t>
   </si>
   <si>
-    <t>PCTPT</t>
-  </si>
-  <si>
     <t>Actual Treatment</t>
   </si>
   <si>
@@ -541,9 +537,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>Analysis Population Indicators</t>
-  </si>
-  <si>
     <t>Description of Actual Arm</t>
   </si>
   <si>
@@ -746,19 +739,13 @@
   </si>
   <si>
     <t>Sequence number of dose</t>
-  </si>
-  <si>
-    <t>EXTDOSE</t>
-  </si>
-  <si>
-    <t>Total dose (mg) at the visit level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,11 +909,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1309,7 +1291,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1349,11 +1331,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1734,1235 +1715,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I60"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>1</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>1</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>1</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>1</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>1</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>1</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
-        <v>1</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>1</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>1</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
-        <v>1</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>1</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
-        <v>1</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
-        <v>1</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
-        <v>1</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>1</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
-        <v>2</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8">
-        <v>2</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8">
-        <v>2</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
-        <v>2</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
-        <v>2</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
-        <v>2</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
-        <v>2</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
-        <v>2</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8">
-        <v>2</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
-        <v>2</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
-        <v>2</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
-        <v>2</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
-        <v>2</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>2</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
-        <v>2</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
-        <v>2</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
-        <v>2</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
-        <v>2</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
-        <v>2</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8">
-        <v>2</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8">
-        <v>2</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8">
-        <v>2</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
-        <v>2</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8">
-        <v>2</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
-        <v>2</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="8">
-        <v>2</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
-        <v>2</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8">
-        <v>2</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8">
-        <v>3</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="8">
-        <v>3</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
-        <v>3</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8">
-        <v>3</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8">
-        <v>3</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="8"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="8"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F60" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,19 +1735,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="F1" s="13"/>
     </row>
@@ -3008,7 +1765,7 @@
         <v>86</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="13"/>
     </row>
@@ -3023,10 +1780,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F3" s="13"/>
     </row>
@@ -3041,10 +1798,10 @@
         <v>56</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F4" s="13"/>
     </row>
@@ -3059,10 +1816,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F5" s="13"/>
     </row>
@@ -3074,13 +1831,13 @@
         <v>105</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F6" s="13"/>
     </row>
@@ -3098,7 +1855,7 @@
         <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F7" s="13"/>
     </row>
@@ -3113,10 +1870,10 @@
         <v>35</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F8" s="13"/>
     </row>
@@ -3134,7 +1891,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" s="13"/>
     </row>
@@ -3149,10 +1906,10 @@
         <v>41</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="13"/>
     </row>
@@ -3170,7 +1927,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="13"/>
     </row>
@@ -3185,10 +1942,10 @@
         <v>38</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" s="13"/>
     </row>
@@ -3203,10 +1960,10 @@
         <v>55</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F13" s="13"/>
     </row>
@@ -3221,10 +1978,10 @@
         <v>30</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F14" s="13"/>
     </row>
@@ -3239,10 +1996,10 @@
         <v>32</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F15" s="13"/>
     </row>
@@ -3257,10 +2014,10 @@
         <v>47</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F16" s="13"/>
     </row>
@@ -3278,7 +2035,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" s="13"/>
     </row>
@@ -3290,13 +2047,13 @@
         <v>105</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F18" s="13"/>
     </row>
@@ -3308,13 +2065,13 @@
         <v>105</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="E19" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F19" s="13"/>
     </row>
@@ -3326,13 +2083,13 @@
         <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>187</v>
+        <v>176</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>185</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3343,13 +2100,13 @@
         <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3360,13 +2117,13 @@
         <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3377,13 +2134,13 @@
         <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3394,13 +2151,13 @@
         <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3411,13 +2168,13 @@
         <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3426,7 +2183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -3448,19 +2205,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3477,7 +2234,7 @@
         <v>86</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3494,7 +2251,7 @@
         <v>126</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3508,10 +2265,10 @@
         <v>48</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3525,10 +2282,10 @@
         <v>49</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3542,10 +2299,10 @@
         <v>17</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F6" s="9"/>
     </row>
@@ -3560,10 +2317,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3580,7 +2337,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3594,10 +2351,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3611,10 +2368,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3628,10 +2385,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F11" s="9"/>
     </row>
@@ -3649,7 +2406,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3660,13 +2417,13 @@
         <v>105</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F13" s="9"/>
     </row>
@@ -3684,7 +2441,7 @@
         <v>112</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F14" s="9"/>
     </row>
@@ -3695,14 +2452,14 @@
       <c r="B15" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3716,10 +2473,10 @@
         <v>13</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3733,10 +2490,10 @@
         <v>84</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3747,13 +2504,13 @@
         <v>105</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>239</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3762,12 +2519,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A16:XFD17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,19 +2539,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
         <v>155</v>
       </c>
-      <c r="B1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>156</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>157</v>
-      </c>
-      <c r="E1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3811,7 +2568,7 @@
         <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3828,7 +2585,7 @@
         <v>126</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3842,10 +2599,10 @@
         <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3859,10 +2616,10 @@
         <v>54</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -3874,13 +2631,13 @@
         <v>105</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3894,10 +2651,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3911,10 +2668,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F8" s="4"/>
     </row>
@@ -3932,7 +2689,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3943,13 +2700,13 @@
         <v>105</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -3960,14 +2717,14 @@
       <c r="B11" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>127</v>
+      <c r="C11" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3984,7 +2741,7 @@
         <v>112</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -4002,7 +2759,7 @@
         <v>113</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -4017,10 +2774,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4034,10 +2791,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F15" s="6"/>
     </row>
@@ -4049,13 +2806,13 @@
         <v>105</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F16" s="6"/>
     </row>
@@ -4067,13 +2824,13 @@
         <v>105</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" s="6"/>
     </row>
@@ -4088,10 +2845,10 @@
         <v>25</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F18" s="4"/>
     </row>
@@ -4109,7 +2866,7 @@
         <v>121</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F19" s="4"/>
     </row>
@@ -4124,10 +2881,10 @@
         <v>100</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -4135,12 +2892,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037B2CA-8556-415F-8A2F-2F4FB3FA0E24}">
-  <dimension ref="A1:F58"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,27 +2907,31 @@
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>158</v>
-      </c>
       <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -4184,11 +2945,14 @@
         <v>107</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -4199,14 +2963,17 @@
         <v>108</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -4220,11 +2987,14 @@
         <v>110</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -4232,35 +3002,41 @@
         <v>105</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>1</v>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -4268,35 +3044,41 @@
         <v>105</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="8"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -4304,35 +3086,41 @@
         <v>105</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>7</v>
+        <v>165</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>1</v>
       </c>
@@ -4340,17 +3128,20 @@
         <v>105</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>165</v>
+        <v>116</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="8"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -4358,17 +3149,20 @@
         <v>105</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>169</v>
       </c>
       <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>1</v>
       </c>
@@ -4376,17 +3170,20 @@
         <v>105</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>169</v>
       </c>
       <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -4394,53 +3191,63 @@
         <v>105</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>1</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="8"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="8"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>1</v>
       </c>
@@ -4448,107 +3255,125 @@
         <v>105</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
-        <v>1</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
-        <v>1</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="8"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>1</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
-        <v>1</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>1</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>1</v>
       </c>
@@ -4556,17 +3381,20 @@
         <v>105</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>168</v>
       </c>
       <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>1</v>
       </c>
@@ -4574,17 +3402,20 @@
         <v>105</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>1</v>
       </c>
@@ -4592,71 +3423,83 @@
         <v>105</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>240</v>
+        <v>28</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>1</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>1</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>1</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
-        <v>1</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
-        <v>1</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
-        <v>1</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>1</v>
       </c>
@@ -4664,17 +3507,20 @@
         <v>105</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>163</v>
+        <v>40</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>1</v>
       </c>
@@ -4682,17 +3528,20 @@
         <v>105</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>169</v>
       </c>
       <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>1</v>
       </c>
@@ -4700,423 +3549,595 @@
         <v>105</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>1</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>2</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>2</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>2</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>2</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>2</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>2</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>2</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>2</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <v>2</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>2</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>2</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
+        <v>2</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
+        <v>2</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
-        <v>1</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="13"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
-        <v>1</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
-        <v>1</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
-        <v>1</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>1</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
-        <v>1</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F37" s="13"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
-        <v>1</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" s="13"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
-        <v>1</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
-        <v>1</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
-        <v>1</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F41" s="13"/>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8">
-        <v>1</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F42" s="13"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8">
-        <v>1</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F43" s="13"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8">
-        <v>1</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F44" s="13"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
-        <v>3</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8">
-        <v>3</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>149</v>
+        <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F48" s="13"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>168</v>
       </c>
       <c r="F49" s="13"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
+        <v>2</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="8">
+        <v>2</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="8">
+        <v>2</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8">
         <v>3</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="B53" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8">
+        <v>3</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D54" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F50" s="13"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="13"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="13"/>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8" t="s">
+        <v>167</v>
+      </c>
       <c r="F54" s="13"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8">
+        <v>3</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>167</v>
+      </c>
       <c r="F55" s="13"/>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="8">
+        <v>3</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="F56" s="13"/>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="13"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
       <c r="F57" s="13"/>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="3"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="8"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="8"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBB57A3-C076-48DB-A987-69C15D972AE4}">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -5131,10 +4152,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5142,7 +4163,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5150,7 +4171,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5158,7 +4179,7 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5166,7 +4187,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5174,7 +4195,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5182,7 +4203,7 @@
         <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5190,7 +4211,7 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5198,7 +4219,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5206,7 +4227,7 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5214,7 +4235,7 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -5222,7 +4243,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -5230,7 +4251,7 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5238,15 +4259,15 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5254,7 +4275,7 @@
         <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5262,7 +4283,7 @@
         <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5270,7 +4291,7 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5278,7 +4299,7 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5286,7 +4307,7 @@
         <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -5294,103 +4315,103 @@
         <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B40" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -5398,7 +4419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F86"/>
   <sheetViews>

</xml_diff>